<commit_message>
Update bespoke unit tests files to remove duplicate font styles.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -58,21 +58,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="3">
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
+  <x:fonts count="1">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>

</xml_diff>

<commit_message>
Fix XLColor equals method (#25)
* Use ToArgb() to compare equality of colors, in order to return TRUE when comparing RGB(FF,FF,FF) to White.
http://stackoverflow.com/questions/8146453/system-drawing-color-equality-operator-doesnt-treat-0xffffffff-as-color-white

* Add test for named color vs RGB

* Update bespoke unit tests files to remove duplicate font styles.

* Set substringo of rich text to Garamond font, instead of Broadway. Broadway probably isn't installed on the AppVeyor server. Garamond is a much more common pre-installed font.

* Disable different font to see if it affects the AppVeyor build.

* Use Courier font for rich text. Hopefully this one is installed on AppVeyor.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -58,21 +58,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="3">
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
+  <x:fonts count="1">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>

</xml_diff>

<commit_message>
Update test files. All .xml files now start with 1, i.e. no more sheet.xml (without digit). Digits now also decimal based, not hexadecimal.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -111,7 +111,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -394,7 +394,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>